<commit_message>
kmeans algorithm image compresion experiment re run
</commit_message>
<xml_diff>
--- a/Experiments/spyder__UCI dataset experiment- FCM-KMeans/third experiment - v2 - Copy.xlsx
+++ b/Experiments/spyder__UCI dataset experiment- FCM-KMeans/third experiment - v2 - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkPlace\github projects\POCS_CLUSTERING\Experiments\spyder__UCI dataset experiment- FCM-KMeans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C88838-33AC-4F08-BE3A-32135E76DFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B71B9BE-6E8F-48BF-8165-E765401CADFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{C67F7B1B-876C-4445-B37D-E1188BFB0A93}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,14 +105,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,14 +127,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -797,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64500F8D-E47F-461B-AEB3-2E83B118DC54}">
   <dimension ref="D6:AE29"/>
   <sheetViews>
-    <sheetView topLeftCell="I11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="X29" sqref="X29"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15:X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,6 +1290,9 @@
       <c r="E14">
         <v>0.56041666666666601</v>
       </c>
+      <c r="F14">
+        <v>0.50595238095238004</v>
+      </c>
       <c r="G14" s="2">
         <v>0.58601190476190401</v>
       </c>
@@ -1311,6 +1305,9 @@
       <c r="L14">
         <v>3.4065357101045697E-2</v>
       </c>
+      <c r="M14">
+        <v>1.5291943546029901E-2</v>
+      </c>
       <c r="N14" s="2">
         <v>4.4273271741570502E-2</v>
       </c>
@@ -1324,7 +1321,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>0.505</v>
       </c>
       <c r="W14">
         <v>0.56599999999999995</v>
@@ -1339,7 +1336,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="AC14">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AD14">
         <v>0.06</v>
@@ -1358,7 +1355,7 @@
       </c>
       <c r="F15">
         <f t="shared" ref="F15:H15" si="0">AVERAGE(F7:F14)</f>
-        <v>0.72780641608990126</v>
+        <v>0.70007466169771115</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -1377,7 +1374,7 @@
       </c>
       <c r="M15">
         <f t="shared" ref="M15:O15" si="1">AVERAGE(M7:M14)</f>
-        <v>2.6674840188561845E-2</v>
+        <v>2.5251978108245351E-2</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
@@ -1394,7 +1391,7 @@
         <v>0.7</v>
       </c>
       <c r="V15">
-        <v>0.72699999999999998</v>
+        <v>0.7</v>
       </c>
       <c r="W15">
         <v>0.71799999999999997</v>
@@ -1409,7 +1406,7 @@
         <v>3.9E-2</v>
       </c>
       <c r="AC15">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AD15">
         <v>1.7999999999999999E-2</v>
@@ -1515,7 +1512,7 @@
         <f t="shared" si="4"/>
         <v>0.889 ± 0.003</v>
       </c>
-      <c r="X21" s="4" t="str">
+      <c r="X21" t="str">
         <f t="shared" si="4"/>
         <v>0.89 ± 0.003</v>
       </c>
@@ -1574,7 +1571,7 @@
         <f t="shared" si="4"/>
         <v>0.954 ± 0.002</v>
       </c>
-      <c r="X22" s="4" t="str">
+      <c r="X22" t="str">
         <f t="shared" si="4"/>
         <v>0.966 ± 0</v>
       </c>
@@ -1633,7 +1630,7 @@
         <f t="shared" si="4"/>
         <v>0.892 ± 0.004</v>
       </c>
-      <c r="X23" s="4" t="str">
+      <c r="X23" t="str">
         <f t="shared" si="4"/>
         <v>0.893 ± 0.003</v>
       </c>
@@ -1688,7 +1685,7 @@
         <f t="shared" si="4"/>
         <v>0.699 ± 0.006</v>
       </c>
-      <c r="W24" s="4" t="str">
+      <c r="W24" t="str">
         <f t="shared" si="4"/>
         <v>0.708 ± 0.002</v>
       </c>
@@ -1751,7 +1748,7 @@
         <f t="shared" si="4"/>
         <v>0.549 ± 0.009</v>
       </c>
-      <c r="X25" s="4" t="str">
+      <c r="X25" t="str">
         <f t="shared" si="4"/>
         <v>0.552 ± 0.012</v>
       </c>
@@ -1810,7 +1807,7 @@
         <f t="shared" si="4"/>
         <v>0.67 ± 0.008</v>
       </c>
-      <c r="X26" s="4" t="str">
+      <c r="X26" t="str">
         <f t="shared" si="4"/>
         <v>0.679 ± 0</v>
       </c>
@@ -1869,7 +1866,7 @@
         <f t="shared" si="4"/>
         <v>0.52 ± 0.055</v>
       </c>
-      <c r="X27" s="4" t="str">
+      <c r="X27" t="str">
         <f t="shared" si="4"/>
         <v>0.534 ± 0.016</v>
       </c>
@@ -1884,7 +1881,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.505</v>
       </c>
       <c r="G28">
         <f t="shared" si="5"/>
@@ -1903,7 +1900,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="N28">
         <f t="shared" si="6"/>
@@ -1922,13 +1919,13 @@
       </c>
       <c r="V28" t="str">
         <f t="shared" si="4"/>
-        <v>0 ± 0</v>
+        <v>0.505 ± 0.015</v>
       </c>
       <c r="W28" t="str">
         <f t="shared" si="4"/>
         <v>0.566 ± 0.06</v>
       </c>
-      <c r="X28" s="4" t="str">
+      <c r="X28" t="str">
         <f t="shared" si="4"/>
         <v>0.586 ± 0.044</v>
       </c>
@@ -1943,7 +1940,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="5"/>
-        <v>0.72699999999999998</v>
+        <v>0.7</v>
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
@@ -1962,7 +1959,7 @@
       </c>
       <c r="M29">
         <f t="shared" ref="M29:O29" si="8">TRUNC(M15,3)</f>
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="N29">
         <f t="shared" si="8"/>
@@ -1981,13 +1978,13 @@
       </c>
       <c r="V29" t="str">
         <f t="shared" si="4"/>
-        <v>0.727 ± 0.026</v>
+        <v>0.7 ± 0.025</v>
       </c>
       <c r="W29" t="str">
         <f t="shared" si="4"/>
         <v>0.718 ± 0.018</v>
       </c>
-      <c r="X29" s="4" t="str">
+      <c r="X29" t="str">
         <f t="shared" si="4"/>
         <v>0.726 ± 0.01</v>
       </c>
@@ -2002,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F284CF2-BF17-4BC2-8BFD-5C51241DD11B}">
   <dimension ref="D6:AD29"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W29" sqref="W29"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15:W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2505,6 +2502,9 @@
       <c r="E14">
         <v>0.83937111915914397</v>
       </c>
+      <c r="F14">
+        <v>0.85851505746742995</v>
+      </c>
       <c r="G14" s="2">
         <v>0.84627859153265494</v>
       </c>
@@ -2517,6 +2517,9 @@
       <c r="L14">
         <v>3.4679865794872297E-2</v>
       </c>
+      <c r="M14">
+        <v>1.3447809647372E-2</v>
+      </c>
       <c r="N14" s="2">
         <v>4.51472667952975E-2</v>
       </c>
@@ -2530,7 +2533,7 @@
         <v>0.83899999999999997</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="V14">
         <v>0.83299999999999996</v>
@@ -2545,7 +2548,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="AB14">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AC14">
         <v>5.2999999999999999E-2</v>
@@ -2564,7 +2567,7 @@
       </c>
       <c r="F15">
         <f t="shared" ref="F15:H15" si="0">AVERAGE(F7:F14)</f>
-        <v>0.74398303483016603</v>
+        <v>0.75829953765982394</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -2583,7 +2586,7 @@
       </c>
       <c r="M15">
         <f t="shared" ref="M15:O15" si="1">AVERAGE(M7:M14)</f>
-        <v>2.8941008859063984E-2</v>
+        <v>2.7004358957602486E-2</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
@@ -2600,7 +2603,7 @@
         <v>0.75</v>
       </c>
       <c r="U15">
-        <v>0.74299999999999999</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="V15">
         <v>0.76100000000000001</v>
@@ -2615,7 +2618,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="AB15">
-        <v>2.8000000000000001E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AC15">
         <v>2.5999999999999999E-2</v>
@@ -2704,15 +2707,15 @@
       <c r="S21" t="s">
         <v>4</v>
       </c>
-      <c r="T21" t="str">
+      <c r="T21" s="4" t="str">
         <f>CONCATENATE(T7," ± ",AA7)</f>
         <v>0.829 ± 0.145</v>
       </c>
-      <c r="U21" t="str">
+      <c r="U21" s="4" t="str">
         <f t="shared" ref="U21:W29" si="4">CONCATENATE(U7," ± ",AB7)</f>
         <v>0.868 ± 0.101</v>
       </c>
-      <c r="V21" t="str">
+      <c r="V21" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.901 ± 0.004</v>
       </c>
@@ -2763,15 +2766,15 @@
       <c r="S22" t="s">
         <v>13</v>
       </c>
-      <c r="T22" t="str">
+      <c r="T22" s="4" t="str">
         <f t="shared" ref="T22:T29" si="7">CONCATENATE(T8," ± ",AA8)</f>
         <v>0.961 ± 0</v>
       </c>
-      <c r="U22" t="str">
+      <c r="U22" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.956 ± 0</v>
       </c>
-      <c r="V22" t="str">
+      <c r="V22" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.954 ± 0.002</v>
       </c>
@@ -2822,15 +2825,15 @@
       <c r="S23" t="s">
         <v>6</v>
       </c>
-      <c r="T23" t="str">
+      <c r="T23" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0.867 ± 0.006</v>
       </c>
-      <c r="U23" t="str">
+      <c r="U23" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.89 ± 0.001</v>
       </c>
-      <c r="V23" t="str">
+      <c r="V23" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.897 ± 0.003</v>
       </c>
@@ -2885,15 +2888,15 @@
         <f t="shared" si="7"/>
         <v>0.743 ± 0.013</v>
       </c>
-      <c r="U24" t="str">
+      <c r="U24" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.727 ± 0.006</v>
       </c>
-      <c r="V24" t="str">
+      <c r="V24" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.734 ± 0.001</v>
       </c>
-      <c r="W24" t="str">
+      <c r="W24" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.731 ± 0.001</v>
       </c>
@@ -2940,15 +2943,15 @@
       <c r="S25" t="s">
         <v>8</v>
       </c>
-      <c r="T25" t="str">
+      <c r="T25" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0.549 ± 0.007</v>
       </c>
-      <c r="U25" t="str">
+      <c r="U25" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.545 ± 0.019</v>
       </c>
-      <c r="V25" t="str">
+      <c r="V25" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.55 ± 0.005</v>
       </c>
@@ -2999,15 +3002,15 @@
       <c r="S26" t="s">
         <v>9</v>
       </c>
-      <c r="T26" t="str">
+      <c r="T26" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0.71 ± 0.044</v>
       </c>
-      <c r="U26" t="str">
+      <c r="U26" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.682 ± 0.063</v>
       </c>
-      <c r="V26" t="str">
+      <c r="V26" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.716 ± 0.007</v>
       </c>
@@ -3058,7 +3061,7 @@
       <c r="S27" t="s">
         <v>10</v>
       </c>
-      <c r="T27" t="str">
+      <c r="T27" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0.504 ± 0.035</v>
       </c>
@@ -3066,11 +3069,11 @@
         <f t="shared" si="4"/>
         <v>0.537 ± 0.009</v>
       </c>
-      <c r="V27" t="str">
+      <c r="V27" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.5 ± 0.131</v>
       </c>
-      <c r="W27" t="str">
+      <c r="W27" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.515 ± 0.027</v>
       </c>
@@ -3085,7 +3088,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="G28">
         <f t="shared" si="5"/>
@@ -3104,7 +3107,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="N28">
         <f t="shared" si="6"/>
@@ -3117,15 +3120,15 @@
       <c r="S28" t="s">
         <v>11</v>
       </c>
-      <c r="T28" t="str">
+      <c r="T28" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0.839 ± 0.034</v>
       </c>
-      <c r="U28" t="str">
-        <f t="shared" si="4"/>
-        <v>0 ± 0</v>
-      </c>
-      <c r="V28" t="str">
+      <c r="U28" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>0.858 ± 0.013</v>
+      </c>
+      <c r="V28" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.833 ± 0.053</v>
       </c>
@@ -3144,7 +3147,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="5"/>
-        <v>0.74299999999999999</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
@@ -3163,7 +3166,7 @@
       </c>
       <c r="M29">
         <f t="shared" si="6"/>
-        <v>2.8000000000000001E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="N29">
         <f t="shared" si="6"/>
@@ -3176,15 +3179,15 @@
       <c r="S29" t="s">
         <v>12</v>
       </c>
-      <c r="T29" t="str">
+      <c r="T29" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0.75 ± 0.035</v>
       </c>
-      <c r="U29" t="str">
-        <f t="shared" si="4"/>
-        <v>0.743 ± 0.028</v>
-      </c>
-      <c r="V29" t="str">
+      <c r="U29" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>0.758 ± 0.027</v>
+      </c>
+      <c r="V29" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.761 ± 0.026</v>
       </c>
@@ -3195,6 +3198,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3202,8 +3206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43FD1DA-214B-4C4E-82FB-B9F1A1F290CA}">
   <dimension ref="D6:AC29"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15:AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,6 +3709,9 @@
       <c r="E14">
         <v>0.56041666666666601</v>
       </c>
+      <c r="F14">
+        <v>0.50595238095238004</v>
+      </c>
       <c r="G14" s="2">
         <v>0.58601190476190401</v>
       </c>
@@ -3717,6 +3724,9 @@
       <c r="L14">
         <v>3.4065357101045697E-2</v>
       </c>
+      <c r="M14">
+        <v>1.5291943546029901E-2</v>
+      </c>
       <c r="N14" s="2">
         <v>4.4273271741570502E-2</v>
       </c>
@@ -3730,7 +3740,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>0.505</v>
       </c>
       <c r="U14">
         <v>0.56599999999999995</v>
@@ -3745,7 +3755,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AB14">
         <v>0.06</v>
@@ -3764,7 +3774,7 @@
       </c>
       <c r="F15">
         <f t="shared" ref="F15:H15" si="0">AVERAGE(F7:F14)</f>
-        <v>0.72780641608990126</v>
+        <v>0.70007466169771115</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -3783,7 +3793,7 @@
       </c>
       <c r="M15">
         <f t="shared" ref="M15:O15" si="1">AVERAGE(M7:M14)</f>
-        <v>2.6674840188561845E-2</v>
+        <v>2.5251978108245351E-2</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
@@ -3800,7 +3810,7 @@
         <v>0.7</v>
       </c>
       <c r="T15">
-        <v>0.72699999999999998</v>
+        <v>0.7</v>
       </c>
       <c r="U15">
         <v>0.71799999999999997</v>
@@ -3815,7 +3825,7 @@
         <v>3.9E-2</v>
       </c>
       <c r="AA15">
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AB15">
         <v>1.7999999999999999E-2</v>
@@ -3916,7 +3926,7 @@
         <f t="shared" si="4"/>
         <v>0.889 ± 0.003</v>
       </c>
-      <c r="V21" s="4" t="str">
+      <c r="V21" t="str">
         <f t="shared" si="4"/>
         <v>0.89 ± 0.003</v>
       </c>
@@ -3975,7 +3985,7 @@
         <f t="shared" si="4"/>
         <v>0.954 ± 0.002</v>
       </c>
-      <c r="V22" s="4" t="str">
+      <c r="V22" t="str">
         <f t="shared" si="4"/>
         <v>0.966 ± 0</v>
       </c>
@@ -4034,7 +4044,7 @@
         <f t="shared" si="4"/>
         <v>0.892 ± 0.004</v>
       </c>
-      <c r="V23" s="4" t="str">
+      <c r="V23" t="str">
         <f t="shared" si="4"/>
         <v>0.893 ± 0.003</v>
       </c>
@@ -4093,7 +4103,7 @@
         <f t="shared" si="4"/>
         <v>0.708 ± 0.002</v>
       </c>
-      <c r="V24" s="4" t="str">
+      <c r="V24" t="str">
         <f t="shared" si="4"/>
         <v>0.707 ± 0.001</v>
       </c>
@@ -4140,15 +4150,15 @@
       <c r="R25" t="s">
         <v>8</v>
       </c>
-      <c r="S25" s="5" t="str">
+      <c r="S25" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0.544 ± 0.007</v>
       </c>
-      <c r="T25" t="str">
+      <c r="T25" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.541 ± 0.02</v>
       </c>
-      <c r="U25" t="str">
+      <c r="U25" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0.549 ± 0.009</v>
       </c>
@@ -4211,7 +4221,7 @@
         <f t="shared" si="4"/>
         <v>0.67 ± 0.008</v>
       </c>
-      <c r="V26" s="4" t="str">
+      <c r="V26" t="str">
         <f t="shared" si="4"/>
         <v>0.679 ± 0</v>
       </c>
@@ -4270,7 +4280,7 @@
         <f t="shared" si="4"/>
         <v>0.52 ± 0.055</v>
       </c>
-      <c r="V27" s="4" t="str">
+      <c r="V27" t="str">
         <f t="shared" si="4"/>
         <v>0.534 ± 0.016</v>
       </c>
@@ -4285,7 +4295,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.505</v>
       </c>
       <c r="G28">
         <f t="shared" si="5"/>
@@ -4304,7 +4314,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="N28">
         <f t="shared" si="6"/>
@@ -4323,13 +4333,13 @@
       </c>
       <c r="T28" t="str">
         <f t="shared" si="4"/>
-        <v>0 ± 0</v>
+        <v>0.505 ± 0.015</v>
       </c>
       <c r="U28" t="str">
         <f t="shared" si="4"/>
         <v>0.566 ± 0.06</v>
       </c>
-      <c r="V28" s="4" t="str">
+      <c r="V28" t="str">
         <f t="shared" si="4"/>
         <v>0.586 ± 0.044</v>
       </c>
@@ -4344,7 +4354,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="5"/>
-        <v>0.72699999999999998</v>
+        <v>0.7</v>
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
@@ -4363,7 +4373,7 @@
       </c>
       <c r="M29">
         <f t="shared" si="6"/>
-        <v>2.5999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="N29">
         <f t="shared" si="6"/>
@@ -4382,13 +4392,13 @@
       </c>
       <c r="T29" t="str">
         <f t="shared" si="4"/>
-        <v>0.727 ± 0.026</v>
+        <v>0.7 ± 0.025</v>
       </c>
       <c r="U29" t="str">
         <f t="shared" si="4"/>
         <v>0.718 ± 0.018</v>
       </c>
-      <c r="V29" s="4" t="str">
+      <c r="V29" t="str">
         <f t="shared" si="4"/>
         <v>0.726 ± 0.01</v>
       </c>
@@ -4402,8 +4412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7165F1A-F55C-47C8-8B67-391CF33F6286}">
   <dimension ref="D6:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15:V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4905,6 +4915,9 @@
       <c r="E14">
         <v>0.63506021884279196</v>
       </c>
+      <c r="F14">
+        <v>0.59619473916472698</v>
+      </c>
       <c r="G14" s="2">
         <v>0.65841052229660801</v>
       </c>
@@ -4917,6 +4930,9 @@
       <c r="L14">
         <v>4.26770500476105E-2</v>
       </c>
+      <c r="M14">
+        <v>4.9361028325504899E-3</v>
+      </c>
       <c r="N14" s="2">
         <v>4.6030307161245697E-2</v>
       </c>
@@ -4930,7 +4946,7 @@
         <v>0.63500000000000001</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="U14">
         <v>0.63700000000000001</v>
@@ -4945,7 +4961,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AB14">
         <v>6.5000000000000002E-2</v>
@@ -4964,7 +4980,7 @@
       </c>
       <c r="F15">
         <f t="shared" ref="F15:H15" si="0">AVERAGE(F7:F14)</f>
-        <v>0.72723742635655786</v>
+        <v>0.71085709045757905</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -4983,7 +4999,7 @@
       </c>
       <c r="M15">
         <f t="shared" ref="M15:O15" si="1">AVERAGE(M7:M14)</f>
-        <v>2.9463553271256625E-2</v>
+        <v>2.6397621966418358E-2</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
@@ -5000,7 +5016,7 @@
         <v>0.70399999999999996</v>
       </c>
       <c r="T15">
-        <v>0.72699999999999998</v>
+        <v>0.71</v>
       </c>
       <c r="U15">
         <v>0.72199999999999998</v>
@@ -5015,7 +5031,7 @@
         <v>0.05</v>
       </c>
       <c r="AA15">
-        <v>2.9000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="AB15">
         <v>2.3E-2</v>
@@ -5109,14 +5125,14 @@
         <v>0.804 ± 0.168</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" ref="T21:V29" si="4">CONCATENATE(T7," ± ",AA7)</f>
+        <f t="shared" ref="T21:V21" si="4">CONCATENATE(T7," ± ",AA7)</f>
         <v>0.851 ± 0.11</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" si="4"/>
         <v>0.887 ± 0.003</v>
       </c>
-      <c r="V21" s="4" t="str">
+      <c r="V21" t="str">
         <f t="shared" si="4"/>
         <v>0.888 ± 0.003</v>
       </c>
@@ -5168,15 +5184,15 @@
         <v>0.96 ± 0</v>
       </c>
       <c r="T22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="T22:V29" si="7">CONCATENATE(T8," ± ",AA8)</f>
         <v>0.955 ± 0</v>
       </c>
       <c r="U22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.954 ± 0.002</v>
       </c>
-      <c r="V22" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V22" t="str">
+        <f t="shared" si="7"/>
         <v>0.966 ± 0</v>
       </c>
     </row>
@@ -5223,19 +5239,19 @@
         <v>6</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" ref="S22:S29" si="7">CONCATENATE(S9," ± ",Z9)</f>
+        <f t="shared" ref="S23:S29" si="8">CONCATENATE(S9," ± ",Z9)</f>
         <v>0.864 ± 0.007</v>
       </c>
       <c r="T23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.886 ± 0.001</v>
       </c>
       <c r="U23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.892 ± 0.004</v>
       </c>
-      <c r="V23" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V23" t="str">
+        <f t="shared" si="7"/>
         <v>0.893 ± 0.003</v>
       </c>
     </row>
@@ -5282,19 +5298,19 @@
         <v>7</v>
       </c>
       <c r="S24" t="str">
+        <f t="shared" si="8"/>
+        <v>0.675 ± 0.083</v>
+      </c>
+      <c r="T24" t="str">
         <f t="shared" si="7"/>
-        <v>0.675 ± 0.083</v>
-      </c>
-      <c r="T24" t="str">
-        <f t="shared" si="4"/>
         <v>0.704 ± 0.006</v>
       </c>
-      <c r="U24" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="U24" t="str">
+        <f t="shared" si="7"/>
         <v>0.713 ± 0.002</v>
       </c>
-      <c r="V24" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V24" t="str">
+        <f t="shared" si="7"/>
         <v>0.713 ± 0.001</v>
       </c>
     </row>
@@ -5341,19 +5357,19 @@
         <v>8</v>
       </c>
       <c r="S25" t="str">
+        <f t="shared" si="8"/>
+        <v>0.544 ± 0.008</v>
+      </c>
+      <c r="T25" t="str">
         <f t="shared" si="7"/>
-        <v>0.544 ± 0.008</v>
-      </c>
-      <c r="T25" t="str">
-        <f t="shared" si="4"/>
         <v>0.541 ± 0.02</v>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.546 ± 0.004</v>
       </c>
-      <c r="V25" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V25" t="str">
+        <f t="shared" si="7"/>
         <v>0.549 ± 0.007</v>
       </c>
     </row>
@@ -5400,19 +5416,19 @@
         <v>9</v>
       </c>
       <c r="S26" t="str">
+        <f t="shared" si="8"/>
+        <v>0.67 ± 0.067</v>
+      </c>
+      <c r="T26" t="str">
         <f t="shared" si="7"/>
-        <v>0.67 ± 0.067</v>
-      </c>
-      <c r="T26" t="str">
-        <f t="shared" si="4"/>
         <v>0.67 ± 0.051</v>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.683 ± 0.007</v>
       </c>
-      <c r="V26" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V26" t="str">
+        <f t="shared" si="7"/>
         <v>0.695 ± 0</v>
       </c>
     </row>
@@ -5459,19 +5475,19 @@
         <v>10</v>
       </c>
       <c r="S27" t="str">
+        <f t="shared" si="8"/>
+        <v>0.483 ± 0.029</v>
+      </c>
+      <c r="T27" t="str">
         <f t="shared" si="7"/>
-        <v>0.483 ± 0.029</v>
-      </c>
-      <c r="T27" t="str">
-        <f t="shared" si="4"/>
         <v>0.48 ± 0.015</v>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.463 ± 0.095</v>
       </c>
-      <c r="V27" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V27" t="str">
+        <f t="shared" si="7"/>
         <v>0.495 ± 0.021</v>
       </c>
     </row>
@@ -5485,7 +5501,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="G28">
         <f t="shared" si="5"/>
@@ -5504,7 +5520,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="N28">
         <f t="shared" si="6"/>
@@ -5518,19 +5534,19 @@
         <v>11</v>
       </c>
       <c r="S28" t="str">
+        <f t="shared" si="8"/>
+        <v>0.635 ± 0.042</v>
+      </c>
+      <c r="T28" t="str">
         <f t="shared" si="7"/>
-        <v>0.635 ± 0.042</v>
-      </c>
-      <c r="T28" t="str">
-        <f t="shared" si="4"/>
-        <v>0 ± 0</v>
+        <v>0.596 ± 0.004</v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.637 ± 0.065</v>
       </c>
-      <c r="V28" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V28" t="str">
+        <f t="shared" si="7"/>
         <v>0.658 ± 0.046</v>
       </c>
     </row>
@@ -5544,7 +5560,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="5"/>
-        <v>0.72699999999999998</v>
+        <v>0.71</v>
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
@@ -5562,34 +5578,34 @@
         <v>0.05</v>
       </c>
       <c r="M29">
-        <f t="shared" ref="M29:O29" si="8">TRUNC(M15,3)</f>
-        <v>2.9000000000000001E-2</v>
+        <f t="shared" ref="M29:O29" si="9">TRUNC(M15,3)</f>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="N29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.01</v>
       </c>
       <c r="O29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.3E-2</v>
       </c>
       <c r="R29" t="s">
         <v>12</v>
       </c>
       <c r="S29" t="str">
+        <f t="shared" si="8"/>
+        <v>0.704 ± 0.05</v>
+      </c>
+      <c r="T29" t="str">
         <f t="shared" si="7"/>
-        <v>0.704 ± 0.05</v>
-      </c>
-      <c r="T29" t="str">
-        <f t="shared" si="4"/>
-        <v>0.727 ± 0.029</v>
+        <v>0.71 ± 0.026</v>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0.722 ± 0.023</v>
       </c>
-      <c r="V29" s="4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V29" t="str">
+        <f t="shared" si="7"/>
         <v>0.732 ± 0.01</v>
       </c>
     </row>

</xml_diff>